<commit_message>
all documents revised and updated
</commit_message>
<xml_diff>
--- a/Documentation/Agile Gantt chartProjectFinal.xlsx
+++ b/Documentation/Agile Gantt chartProjectFinal.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{684D94CC-A0DE-4247-869E-2F69DEFAB9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D8E7939-DD5D-4F3E-86AF-12865DB85DAD}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{684D94CC-A0DE-4247-869E-2F69DEFAB9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1650A066-8D07-41B2-81B9-57C90560F8C7}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -511,7 +511,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -592,6 +592,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1245,9 +1251,6 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1284,6 +1287,9 @@
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Accent3" xfId="11" builtinId="37"/>
@@ -1299,760 +1305,36 @@
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="89">
+  <dxfs count="84">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </left>
-        <right style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="7" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="7" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="6"/>
-        </left>
-        <right style="thin">
-          <color theme="6"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-      </border>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
         <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
-      <border>
-        <left style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </left>
-        <right style="thin">
-          <color theme="2" tint="-9.9948118533890809E-2"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="7" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="7" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="6"/>
-        </left>
-        <right style="thin">
-          <color theme="6"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -2323,36 +1605,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
         <color auto="1"/>
         <name val="Calibri"/>
         <family val="2"/>
@@ -2364,6 +1616,251 @@
           <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="2" tint="-9.9948118533890809E-2"/>
+        </left>
+        <right style="thin">
+          <color theme="2" tint="-9.9948118533890809E-2"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="7" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="7" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="6"/>
+        </left>
+        <right style="thin">
+          <color theme="6"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2479,6 +1976,406 @@
           <bgColor theme="1" tint="0.249977111117893"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -2651,21 +2548,21 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Gantt Table Style" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Gantt Table Style" pivot="0" count="4" xr9:uid="{4904D139-63E4-4221-B7C9-C6C5B7A50FAF}">
-      <tableStyleElement type="wholeTable" dxfId="88"/>
-      <tableStyleElement type="headerRow" dxfId="87"/>
-      <tableStyleElement type="firstRowStripe" dxfId="86"/>
-      <tableStyleElement type="secondRowStripe" dxfId="85"/>
+      <tableStyleElement type="wholeTable" dxfId="83"/>
+      <tableStyleElement type="headerRow" dxfId="82"/>
+      <tableStyleElement type="firstRowStripe" dxfId="81"/>
+      <tableStyleElement type="secondRowStripe" dxfId="80"/>
     </tableStyle>
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="84"/>
-      <tableStyleElement type="headerRow" dxfId="83"/>
-      <tableStyleElement type="totalRow" dxfId="82"/>
-      <tableStyleElement type="firstColumn" dxfId="81"/>
-      <tableStyleElement type="lastColumn" dxfId="80"/>
-      <tableStyleElement type="firstRowStripe" dxfId="79"/>
-      <tableStyleElement type="secondRowStripe" dxfId="78"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="77"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="76"/>
+      <tableStyleElement type="wholeTable" dxfId="79"/>
+      <tableStyleElement type="headerRow" dxfId="78"/>
+      <tableStyleElement type="totalRow" dxfId="77"/>
+      <tableStyleElement type="firstColumn" dxfId="76"/>
+      <tableStyleElement type="lastColumn" dxfId="75"/>
+      <tableStyleElement type="firstRowStripe" dxfId="74"/>
+      <tableStyleElement type="secondRowStripe" dxfId="73"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="72"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="71"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2994,7 +2891,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Milestones4352" displayName="Milestones4352" ref="B9:G32" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Milestones4352" displayName="Milestones4352" ref="B9:G32" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="B9:G32" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3004,12 +2901,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{619BF8F6-D0F1-41AD-871D-FE0240C45A93}" name="Milestone description" dataDxfId="73"/>
-    <tableColumn id="2" xr3:uid="{39BD914E-FB02-4352-846C-6D59624DC0B0}" name="Category" dataDxfId="72"/>
-    <tableColumn id="3" xr3:uid="{D274194F-BCA0-44F3-84B2-217254EE241C}" name="Assigned to" dataDxfId="71"/>
-    <tableColumn id="4" xr3:uid="{8385BC6F-56EE-4363-A106-8DB0A1E4EF5A}" name="Progress" dataDxfId="70"/>
-    <tableColumn id="5" xr3:uid="{02926609-7B93-4B6F-BE96-92EC7A949E4B}" name="Start" dataDxfId="69" dataCellStyle="Date"/>
-    <tableColumn id="6" xr3:uid="{8FF9BE8E-04B7-4B39-AC27-D2E534204BC3}" name="Days" dataDxfId="68" dataCellStyle="Comma [0]"/>
+    <tableColumn id="1" xr3:uid="{619BF8F6-D0F1-41AD-871D-FE0240C45A93}" name="Milestone description" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{39BD914E-FB02-4352-846C-6D59624DC0B0}" name="Category" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{D274194F-BCA0-44F3-84B2-217254EE241C}" name="Assigned to" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{8385BC6F-56EE-4363-A106-8DB0A1E4EF5A}" name="Progress" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{02926609-7B93-4B6F-BE96-92EC7A949E4B}" name="Start" dataDxfId="37" dataCellStyle="Date"/>
+    <tableColumn id="6" xr3:uid="{8FF9BE8E-04B7-4B39-AC27-D2E534204BC3}" name="Days" dataDxfId="36" dataCellStyle="Comma [0]"/>
   </tableColumns>
   <tableStyleInfo name="ToDoList" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3021,7 +2918,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0EDB95CA-98FE-4198-8801-690B9B480FDF}" name="Milestones435" displayName="Milestones435" ref="B9:G36" totalsRowShown="0" headerRowDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0EDB95CA-98FE-4198-8801-690B9B480FDF}" name="Milestones435" displayName="Milestones435" ref="B9:G36" totalsRowShown="0" headerRowDxfId="21">
   <autoFilter ref="B9:G36" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3031,9 +2928,9 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6E47A83D-ACD7-4EB6-9B84-5195E813945E}" name="Milestone description" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{529EEF64-D037-4ACF-8CA4-0C10FE2D1FBB}" name="Category" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{711D01BA-2785-403A-9636-CCC7E2ADA584}" name="Assigned to" dataDxfId="64"/>
+    <tableColumn id="1" xr3:uid="{6E47A83D-ACD7-4EB6-9B84-5195E813945E}" name="Milestone description" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{529EEF64-D037-4ACF-8CA4-0C10FE2D1FBB}" name="Category" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{711D01BA-2785-403A-9636-CCC7E2ADA584}" name="Assigned to" dataDxfId="18"/>
     <tableColumn id="4" xr3:uid="{62B00BEF-16BE-4692-B5E2-F287F680F2C1}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{D6D72902-F68F-4E59-A714-AFFF520C647A}" name="Start" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{93E698DE-286F-49ED-AA20-D0C843671DE8}" name="Days" dataCellStyle="Comma [0]"/>
@@ -3048,7 +2945,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{876EA49D-634E-482B-8173-880F7B761E2C}" name="Milestones43524" displayName="Milestones43524" ref="B9:G36" totalsRowShown="0" headerRowDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{876EA49D-634E-482B-8173-880F7B761E2C}" name="Milestones43524" displayName="Milestones43524" ref="B9:G36" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="B9:G36" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3058,9 +2955,9 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{0971B905-713A-4980-8BBC-DF959C2E61F9}" name="Milestone description" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{4492A0B8-068F-4002-9E8D-E1F5FED367F0}" name="Category" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{DF1A764E-7050-4528-B7F9-B6AB99372146}" name="Assigned to" dataDxfId="60"/>
+    <tableColumn id="1" xr3:uid="{0971B905-713A-4980-8BBC-DF959C2E61F9}" name="Milestone description" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{4492A0B8-068F-4002-9E8D-E1F5FED367F0}" name="Category" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{DF1A764E-7050-4528-B7F9-B6AB99372146}" name="Assigned to" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{47C54592-75B0-4C70-BBF8-0F40483670E9}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{663FB5E0-7616-4EA5-B56A-FF069E2E07D7}" name="Start" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{3B766962-C06F-4E12-BE91-12AB93439874}" name="Days" dataCellStyle="Comma [0]"/>
@@ -3513,7 +3410,7 @@
   <dimension ref="A1:BP34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3534,27 +3431,27 @@
     <row r="1" spans="1:68" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:68" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
-      <c r="B2" s="146" t="s">
+      <c r="B2" s="158" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="146"/>
-      <c r="F2" s="146"/>
-      <c r="G2" s="146"/>
-      <c r="H2" s="146"/>
-      <c r="I2" s="147"/>
-      <c r="J2" s="147"/>
-      <c r="K2" s="147"/>
-      <c r="L2" s="147"/>
-      <c r="M2" s="147"/>
-      <c r="N2" s="147"/>
-      <c r="O2" s="148"/>
-      <c r="P2" s="148"/>
-      <c r="Q2" s="148"/>
-      <c r="R2" s="148"/>
-      <c r="S2" s="148"/>
-      <c r="T2" s="148"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="146"/>
+      <c r="J2" s="146"/>
+      <c r="K2" s="146"/>
+      <c r="L2" s="146"/>
+      <c r="M2" s="146"/>
+      <c r="N2" s="146"/>
+      <c r="O2" s="147"/>
+      <c r="P2" s="147"/>
+      <c r="Q2" s="147"/>
+      <c r="R2" s="147"/>
+      <c r="S2" s="147"/>
+      <c r="T2" s="147"/>
       <c r="U2" s="76"/>
       <c r="V2" s="76"/>
       <c r="W2" s="76"/>
@@ -3681,26 +3578,26 @@
         <v>18</v>
       </c>
       <c r="H4" s="84"/>
-      <c r="I4" s="149" t="s">
+      <c r="I4" s="148" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="149"/>
-      <c r="K4" s="149"/>
-      <c r="L4" s="149"/>
+      <c r="J4" s="148"/>
+      <c r="K4" s="148"/>
+      <c r="L4" s="148"/>
       <c r="M4" s="99"/>
-      <c r="N4" s="150" t="s">
+      <c r="N4" s="149" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="150"/>
-      <c r="P4" s="150"/>
-      <c r="Q4" s="150"/>
+      <c r="O4" s="149"/>
+      <c r="P4" s="149"/>
+      <c r="Q4" s="149"/>
       <c r="R4" s="99"/>
-      <c r="S4" s="151" t="s">
+      <c r="S4" s="150" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="151"/>
-      <c r="U4" s="151"/>
-      <c r="V4" s="151"/>
+      <c r="T4" s="150"/>
+      <c r="U4" s="150"/>
+      <c r="V4" s="150"/>
       <c r="W4" s="99"/>
       <c r="X4" s="144" t="s">
         <v>29</v>
@@ -9481,39 +9378,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL17 I19:BL23 I25:BL30 I32:BL32">
-    <cfRule type="expression" dxfId="59" priority="25">
+    <cfRule type="expression" dxfId="70" priority="25">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:AM6">
-    <cfRule type="expression" dxfId="58" priority="28">
+    <cfRule type="expression" dxfId="69" priority="28">
       <formula>I$7&lt;=EOMONTH($I$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:BL6">
-    <cfRule type="expression" dxfId="57" priority="27">
+    <cfRule type="expression" dxfId="68" priority="27">
       <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BL6">
-    <cfRule type="expression" dxfId="56" priority="26">
+    <cfRule type="expression" dxfId="67" priority="26">
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:BL17 I19:BL23 I25:BL30 I32:BL32">
-    <cfRule type="expression" dxfId="55" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="31" stopIfTrue="1">
       <formula>AND($C10="Low Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="32" stopIfTrue="1">
       <formula>AND($C10="High Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="33" stopIfTrue="1">
       <formula>AND($C10="On Track",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="34" stopIfTrue="1">
       <formula>AND($C10="Med Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="35" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9532,24 +9429,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:BL18">
-    <cfRule type="expression" dxfId="45" priority="17">
+    <cfRule type="expression" dxfId="61" priority="17">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:BL18">
-    <cfRule type="expression" dxfId="44" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="20" stopIfTrue="1">
       <formula>AND($C18="Low Risk",I$7&gt;=$F18,I$7&lt;=$F18+$G18-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="21" stopIfTrue="1">
       <formula>AND($C18="High Risk",I$7&gt;=$F18,I$7&lt;=$F18+$G18-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="22" stopIfTrue="1">
       <formula>AND($C18="On Track",I$7&gt;=$F18,I$7&lt;=$F18+$G18-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="23" stopIfTrue="1">
       <formula>AND($C18="Med Risk",I$7&gt;=$F18,I$7&lt;=$F18+$G18-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="24" stopIfTrue="1">
       <formula>AND(LEN($C18)=0,I$7&gt;=$F18,I$7&lt;=$F18+$G18-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9568,24 +9465,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24:BL24">
-    <cfRule type="expression" dxfId="39" priority="9">
+    <cfRule type="expression" dxfId="55" priority="9">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24:BL24">
-    <cfRule type="expression" dxfId="38" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="11" stopIfTrue="1">
       <formula>AND($C24="Low Risk",I$7&gt;=$F24,I$7&lt;=$F24+$G24-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="12" stopIfTrue="1">
       <formula>AND($C24="High Risk",I$7&gt;=$F24,I$7&lt;=$F24+$G24-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="13" stopIfTrue="1">
       <formula>AND($C24="On Track",I$7&gt;=$F24,I$7&lt;=$F24+$G24-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="14" stopIfTrue="1">
       <formula>AND($C24="Med Risk",I$7&gt;=$F24,I$7&lt;=$F24+$G24-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="15" stopIfTrue="1">
       <formula>AND(LEN($C24)=0,I$7&gt;=$F24,I$7&lt;=$F24+$G24-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9604,24 +9501,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31:BL31">
-    <cfRule type="expression" dxfId="33" priority="1">
+    <cfRule type="expression" dxfId="49" priority="1">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31:BL31">
-    <cfRule type="expression" dxfId="32" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="3" stopIfTrue="1">
       <formula>AND($C31="Low Risk",I$7&gt;=$F31,I$7&lt;=$F31+$G31-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="4" stopIfTrue="1">
       <formula>AND($C31="High Risk",I$7&gt;=$F31,I$7&lt;=$F31+$G31-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="5" stopIfTrue="1">
       <formula>AND($C31="On Track",I$7&gt;=$F31,I$7&lt;=$F31+$G31-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="6" stopIfTrue="1">
       <formula>AND($C31="Med Risk",I$7&gt;=$F31,I$7&lt;=$F31+$G31-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="7" stopIfTrue="1">
       <formula>AND(LEN($C31)=0,I$7&gt;=$F31,I$7&lt;=$F31+$G31-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9855,27 +9752,27 @@
     <row r="1" spans="1:68" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:68" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="151" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="152"/>
-      <c r="D2" s="152"/>
-      <c r="E2" s="152"/>
-      <c r="F2" s="152"/>
-      <c r="G2" s="152"/>
-      <c r="H2" s="152"/>
-      <c r="I2" s="153"/>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
-      <c r="L2" s="153"/>
-      <c r="M2" s="153"/>
-      <c r="N2" s="153"/>
-      <c r="O2" s="154"/>
-      <c r="P2" s="155"/>
-      <c r="Q2" s="155"/>
-      <c r="R2" s="155"/>
-      <c r="S2" s="155"/>
-      <c r="T2" s="155"/>
+      <c r="C2" s="151"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="151"/>
+      <c r="F2" s="151"/>
+      <c r="G2" s="151"/>
+      <c r="H2" s="151"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
+      <c r="O2" s="153"/>
+      <c r="P2" s="154"/>
+      <c r="Q2" s="154"/>
+      <c r="R2" s="154"/>
+      <c r="S2" s="154"/>
+      <c r="T2" s="154"/>
       <c r="U2" s="23"/>
       <c r="V2" s="23"/>
       <c r="W2" s="23"/>
@@ -10002,26 +9899,26 @@
         <v>18</v>
       </c>
       <c r="H4" s="32"/>
-      <c r="I4" s="149" t="s">
+      <c r="I4" s="148" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="149"/>
-      <c r="K4" s="149"/>
-      <c r="L4" s="149"/>
+      <c r="J4" s="148"/>
+      <c r="K4" s="148"/>
+      <c r="L4" s="148"/>
       <c r="M4" s="35"/>
-      <c r="N4" s="150" t="s">
+      <c r="N4" s="149" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="150"/>
-      <c r="P4" s="150"/>
-      <c r="Q4" s="150"/>
+      <c r="O4" s="149"/>
+      <c r="P4" s="149"/>
+      <c r="Q4" s="149"/>
       <c r="R4" s="35"/>
-      <c r="S4" s="151" t="s">
+      <c r="S4" s="150" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="151"/>
-      <c r="U4" s="151"/>
-      <c r="V4" s="151"/>
+      <c r="T4" s="150"/>
+      <c r="U4" s="150"/>
+      <c r="V4" s="150"/>
       <c r="W4" s="35"/>
       <c r="X4" s="144" t="s">
         <v>29</v>
@@ -10146,7 +10043,7 @@
       </c>
       <c r="C6" s="39" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">IFERROR(IF(MIN(Milestones435[Start])=0,TODAY(),B11(Milestones435[Start])),TODAY())</f>
-        <v>44706</v>
+        <v>44710</v>
       </c>
       <c r="D6" s="60"/>
       <c r="E6" s="35"/>
@@ -10205,7 +10102,7 @@
       <c r="AQ6" s="112"/>
       <c r="AR6" s="112" t="str">
         <f ca="1">IF(OR(TEXT(AR7,"mmmm")=AK6,TEXT(AR7,"mmmm")=AD6,TEXT(AR7,"mmmm")=W6,TEXT(AR7,"mmmm")=P6),"",TEXT(AR7,"mmmm"))</f>
-        <v/>
+        <v>July</v>
       </c>
       <c r="AS6" s="112"/>
       <c r="AT6" s="112"/>
@@ -10215,7 +10112,7 @@
       <c r="AX6" s="112"/>
       <c r="AY6" s="112" t="str">
         <f ca="1">IF(OR(TEXT(AY7,"mmmm")=AR6,TEXT(AY7,"mmmm")=AK6,TEXT(AY7,"mmmm")=AD6,TEXT(AY7,"mmmm")=W6),"",TEXT(AY7,"mmmm"))</f>
-        <v>July</v>
+        <v/>
       </c>
       <c r="AZ6" s="112"/>
       <c r="BA6" s="112"/>
@@ -10250,227 +10147,227 @@
       <c r="H7" s="38"/>
       <c r="I7" s="114">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>44707</v>
+        <v>44711</v>
       </c>
       <c r="J7" s="19">
         <f ca="1">I7+1</f>
-        <v>44708</v>
+        <v>44712</v>
       </c>
       <c r="K7" s="19">
         <f t="shared" ref="K7:AX7" ca="1" si="0">J7+1</f>
-        <v>44709</v>
+        <v>44713</v>
       </c>
       <c r="L7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44710</v>
+        <v>44714</v>
       </c>
       <c r="M7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44711</v>
+        <v>44715</v>
       </c>
       <c r="N7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44712</v>
+        <v>44716</v>
       </c>
       <c r="O7" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>44713</v>
+        <v>44717</v>
       </c>
       <c r="P7" s="19">
         <f ca="1">O7+1</f>
-        <v>44714</v>
+        <v>44718</v>
       </c>
       <c r="Q7" s="19">
         <f ca="1">P7+1</f>
-        <v>44715</v>
+        <v>44719</v>
       </c>
       <c r="R7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44716</v>
+        <v>44720</v>
       </c>
       <c r="S7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44717</v>
+        <v>44721</v>
       </c>
       <c r="T7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44718</v>
+        <v>44722</v>
       </c>
       <c r="U7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44719</v>
+        <v>44723</v>
       </c>
       <c r="V7" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>44720</v>
+        <v>44724</v>
       </c>
       <c r="W7" s="19">
         <f ca="1">V7+1</f>
-        <v>44721</v>
+        <v>44725</v>
       </c>
       <c r="X7" s="19">
         <f ca="1">W7+1</f>
-        <v>44722</v>
+        <v>44726</v>
       </c>
       <c r="Y7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44723</v>
+        <v>44727</v>
       </c>
       <c r="Z7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44724</v>
+        <v>44728</v>
       </c>
       <c r="AA7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44725</v>
+        <v>44729</v>
       </c>
       <c r="AB7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44726</v>
+        <v>44730</v>
       </c>
       <c r="AC7" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>44727</v>
+        <v>44731</v>
       </c>
       <c r="AD7" s="19">
         <f ca="1">AC7+1</f>
-        <v>44728</v>
+        <v>44732</v>
       </c>
       <c r="AE7" s="19">
         <f ca="1">AD7+1</f>
-        <v>44729</v>
+        <v>44733</v>
       </c>
       <c r="AF7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44730</v>
+        <v>44734</v>
       </c>
       <c r="AG7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44731</v>
+        <v>44735</v>
       </c>
       <c r="AH7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44732</v>
+        <v>44736</v>
       </c>
       <c r="AI7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44733</v>
+        <v>44737</v>
       </c>
       <c r="AJ7" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>44734</v>
+        <v>44738</v>
       </c>
       <c r="AK7" s="19">
         <f ca="1">AJ7+1</f>
-        <v>44735</v>
+        <v>44739</v>
       </c>
       <c r="AL7" s="19">
         <f ca="1">AK7+1</f>
-        <v>44736</v>
+        <v>44740</v>
       </c>
       <c r="AM7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44737</v>
+        <v>44741</v>
       </c>
       <c r="AN7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44738</v>
+        <v>44742</v>
       </c>
       <c r="AO7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44739</v>
+        <v>44743</v>
       </c>
       <c r="AP7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44740</v>
+        <v>44744</v>
       </c>
       <c r="AQ7" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>44741</v>
+        <v>44745</v>
       </c>
       <c r="AR7" s="19">
         <f ca="1">AQ7+1</f>
-        <v>44742</v>
+        <v>44746</v>
       </c>
       <c r="AS7" s="19">
         <f ca="1">AR7+1</f>
-        <v>44743</v>
+        <v>44747</v>
       </c>
       <c r="AT7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44744</v>
+        <v>44748</v>
       </c>
       <c r="AU7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44745</v>
+        <v>44749</v>
       </c>
       <c r="AV7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44746</v>
+        <v>44750</v>
       </c>
       <c r="AW7" s="19">
         <f t="shared" ca="1" si="0"/>
-        <v>44747</v>
+        <v>44751</v>
       </c>
       <c r="AX7" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>44748</v>
+        <v>44752</v>
       </c>
       <c r="AY7" s="19">
         <f ca="1">AX7+1</f>
-        <v>44749</v>
+        <v>44753</v>
       </c>
       <c r="AZ7" s="19">
         <f ca="1">AY7+1</f>
-        <v>44750</v>
+        <v>44754</v>
       </c>
       <c r="BA7" s="19">
         <f t="shared" ref="BA7:BE7" ca="1" si="1">AZ7+1</f>
-        <v>44751</v>
+        <v>44755</v>
       </c>
       <c r="BB7" s="19">
         <f t="shared" ca="1" si="1"/>
-        <v>44752</v>
+        <v>44756</v>
       </c>
       <c r="BC7" s="19">
         <f t="shared" ca="1" si="1"/>
-        <v>44753</v>
+        <v>44757</v>
       </c>
       <c r="BD7" s="19">
         <f t="shared" ca="1" si="1"/>
-        <v>44754</v>
+        <v>44758</v>
       </c>
       <c r="BE7" s="72">
         <f t="shared" ca="1" si="1"/>
-        <v>44755</v>
+        <v>44759</v>
       </c>
       <c r="BF7" s="19">
         <f ca="1">BE7+1</f>
-        <v>44756</v>
+        <v>44760</v>
       </c>
       <c r="BG7" s="19">
         <f ca="1">BF7+1</f>
-        <v>44757</v>
+        <v>44761</v>
       </c>
       <c r="BH7" s="19">
         <f t="shared" ref="BH7:BL7" ca="1" si="2">BG7+1</f>
-        <v>44758</v>
+        <v>44762</v>
       </c>
       <c r="BI7" s="19">
         <f t="shared" ca="1" si="2"/>
-        <v>44759</v>
+        <v>44763</v>
       </c>
       <c r="BJ7" s="19">
         <f t="shared" ca="1" si="2"/>
-        <v>44760</v>
+        <v>44764</v>
       </c>
       <c r="BK7" s="19">
         <f t="shared" ca="1" si="2"/>
-        <v>44761</v>
+        <v>44765</v>
       </c>
       <c r="BL7" s="20">
         <f t="shared" ca="1" si="2"/>
-        <v>44762</v>
+        <v>44766</v>
       </c>
       <c r="BM7" s="35"/>
     </row>
@@ -10564,227 +10461,227 @@
       <c r="H9" s="55"/>
       <c r="I9" s="43" t="str">
         <f t="shared" ref="I9:BL9" ca="1" si="3">LEFT(TEXT(I7,"ddd"),1)</f>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="J9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="K9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="L9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="M9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="N9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="O9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="P9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="Q9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="R9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="S9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="T9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="U9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="V9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="W9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="X9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="Y9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="Z9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AA9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="AB9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AC9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="AD9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AE9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="AF9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="AG9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AH9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="AI9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AJ9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="AK9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AL9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="AM9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="AN9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AO9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="AP9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AQ9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="AR9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AS9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="AT9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="AU9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AV9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="AW9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AX9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="AY9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AZ9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="BA9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="BB9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="BC9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="BD9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="BE9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="BF9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="BG9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="BH9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="BI9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="BJ9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="BK9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="BL9" s="43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="BM9" s="35"/>
     </row>
@@ -11108,7 +11005,7 @@
       </c>
       <c r="F12" s="26">
         <f ca="1">TODAY()</f>
-        <v>44706</v>
+        <v>44710</v>
       </c>
       <c r="G12" s="27">
         <v>3</v>
@@ -11352,7 +11249,7 @@
       <c r="E13" s="25"/>
       <c r="F13" s="26">
         <f ca="1">TODAY()+5</f>
-        <v>44711</v>
+        <v>44715</v>
       </c>
       <c r="G13" s="27">
         <v>1</v>
@@ -11598,7 +11495,7 @@
       </c>
       <c r="F14" s="26">
         <f ca="1">F12-3</f>
-        <v>44703</v>
+        <v>44707</v>
       </c>
       <c r="G14" s="27">
         <v>10</v>
@@ -11842,7 +11739,7 @@
       <c r="E15" s="25"/>
       <c r="F15" s="26">
         <f ca="1">F12+20</f>
-        <v>44726</v>
+        <v>44730</v>
       </c>
       <c r="G15" s="27">
         <v>1</v>
@@ -12088,7 +11985,7 @@
       </c>
       <c r="F16" s="26">
         <f ca="1">F12+6</f>
-        <v>44712</v>
+        <v>44716</v>
       </c>
       <c r="G16" s="27">
         <v>6</v>
@@ -12571,7 +12468,7 @@
       </c>
       <c r="F18" s="26">
         <f ca="1">F12+6</f>
-        <v>44712</v>
+        <v>44716</v>
       </c>
       <c r="G18" s="27">
         <v>13</v>
@@ -12817,7 +12714,7 @@
       </c>
       <c r="F19" s="26">
         <f ca="1">F18+2</f>
-        <v>44714</v>
+        <v>44718</v>
       </c>
       <c r="G19" s="27">
         <v>9</v>
@@ -13063,7 +12960,7 @@
       </c>
       <c r="F20" s="26">
         <f ca="1">F19+5</f>
-        <v>44719</v>
+        <v>44723</v>
       </c>
       <c r="G20" s="27">
         <v>11</v>
@@ -13307,7 +13204,7 @@
       <c r="E21" s="25"/>
       <c r="F21" s="26">
         <f ca="1">F20+2</f>
-        <v>44721</v>
+        <v>44725</v>
       </c>
       <c r="G21" s="27">
         <v>1</v>
@@ -13549,7 +13446,7 @@
       <c r="E22" s="25"/>
       <c r="F22" s="26">
         <f ca="1">F21+1</f>
-        <v>44722</v>
+        <v>44726</v>
       </c>
       <c r="G22" s="27">
         <v>24</v>
@@ -14030,7 +13927,7 @@
       <c r="E24" s="25"/>
       <c r="F24" s="26">
         <f ca="1">F12+15</f>
-        <v>44721</v>
+        <v>44725</v>
       </c>
       <c r="G24" s="27">
         <v>4</v>
@@ -14274,7 +14171,7 @@
       <c r="E25" s="25"/>
       <c r="F25" s="26">
         <f ca="1">F24+3</f>
-        <v>44724</v>
+        <v>44728</v>
       </c>
       <c r="G25" s="27">
         <v>14</v>
@@ -14518,7 +14415,7 @@
       <c r="E26" s="25"/>
       <c r="F26" s="26">
         <f ca="1">F25+15</f>
-        <v>44739</v>
+        <v>44743</v>
       </c>
       <c r="G26" s="27">
         <v>6</v>
@@ -14762,7 +14659,7 @@
       <c r="E27" s="25"/>
       <c r="F27" s="26">
         <f ca="1">F21+22</f>
-        <v>44743</v>
+        <v>44747</v>
       </c>
       <c r="G27" s="27">
         <v>3</v>
@@ -15006,7 +14903,7 @@
       <c r="E28" s="25"/>
       <c r="F28" s="26">
         <f ca="1">F16</f>
-        <v>44712</v>
+        <v>44716</v>
       </c>
       <c r="G28" s="27">
         <v>19</v>
@@ -15485,7 +15382,7 @@
       <c r="E30" s="25"/>
       <c r="F30" s="26">
         <f ca="1">F27+3</f>
-        <v>44746</v>
+        <v>44750</v>
       </c>
       <c r="G30" s="27">
         <v>15</v>
@@ -15727,7 +15624,7 @@
       <c r="E31" s="25"/>
       <c r="F31" s="26">
         <f ca="1">F30+14</f>
-        <v>44760</v>
+        <v>44764</v>
       </c>
       <c r="G31" s="27">
         <v>5</v>
@@ -15971,7 +15868,7 @@
       <c r="E32" s="25"/>
       <c r="F32" s="26">
         <f ca="1">F31+42</f>
-        <v>44802</v>
+        <v>44806</v>
       </c>
       <c r="G32" s="27">
         <v>1</v>
@@ -17015,56 +16912,56 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL36">
-    <cfRule type="expression" dxfId="27" priority="1">
+    <cfRule type="expression" dxfId="35" priority="1">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:AM6">
-    <cfRule type="expression" dxfId="26" priority="4">
+    <cfRule type="expression" dxfId="34" priority="4">
       <formula>I$7&lt;=EOMONTH($I$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:BL6">
-    <cfRule type="expression" dxfId="25" priority="3">
+    <cfRule type="expression" dxfId="33" priority="3">
       <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BL6">
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="32" priority="2">
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:BL35">
-    <cfRule type="expression" dxfId="23" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="7" stopIfTrue="1">
       <formula>AND($C10="Low Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="8" stopIfTrue="1">
       <formula>AND($C10="High Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="9" stopIfTrue="1">
       <formula>AND($C10="On Track",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="10" stopIfTrue="1">
       <formula>AND($C10="Med Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="11" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:BL36">
-    <cfRule type="expression" dxfId="18" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="13" stopIfTrue="1">
       <formula>AND(#REF!="Low Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="14" stopIfTrue="1">
       <formula>AND(#REF!="High Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="15" stopIfTrue="1">
       <formula>AND(#REF!="On Track",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="16" stopIfTrue="1">
       <formula>AND(#REF!="Med Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="17" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17217,27 +17114,27 @@
     <row r="1" spans="1:68" ht="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:68" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
-      <c r="B2" s="156" t="s">
+      <c r="B2" s="155" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
-      <c r="G2" s="156"/>
-      <c r="H2" s="156"/>
-      <c r="I2" s="157"/>
-      <c r="J2" s="157"/>
-      <c r="K2" s="157"/>
-      <c r="L2" s="157"/>
-      <c r="M2" s="157"/>
-      <c r="N2" s="157"/>
-      <c r="O2" s="158"/>
-      <c r="P2" s="158"/>
-      <c r="Q2" s="158"/>
-      <c r="R2" s="158"/>
-      <c r="S2" s="158"/>
-      <c r="T2" s="158"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
+      <c r="F2" s="155"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="155"/>
+      <c r="I2" s="156"/>
+      <c r="J2" s="156"/>
+      <c r="K2" s="156"/>
+      <c r="L2" s="156"/>
+      <c r="M2" s="156"/>
+      <c r="N2" s="156"/>
+      <c r="O2" s="157"/>
+      <c r="P2" s="157"/>
+      <c r="Q2" s="157"/>
+      <c r="R2" s="157"/>
+      <c r="S2" s="157"/>
+      <c r="T2" s="157"/>
       <c r="U2" s="115"/>
       <c r="V2" s="115"/>
       <c r="W2" s="115"/>
@@ -17364,26 +17261,26 @@
         <v>18</v>
       </c>
       <c r="H4" s="84"/>
-      <c r="I4" s="149" t="s">
+      <c r="I4" s="148" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="149"/>
-      <c r="K4" s="149"/>
-      <c r="L4" s="149"/>
+      <c r="J4" s="148"/>
+      <c r="K4" s="148"/>
+      <c r="L4" s="148"/>
       <c r="M4" s="99"/>
-      <c r="N4" s="150" t="s">
+      <c r="N4" s="149" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="150"/>
-      <c r="P4" s="150"/>
-      <c r="Q4" s="150"/>
+      <c r="O4" s="149"/>
+      <c r="P4" s="149"/>
+      <c r="Q4" s="149"/>
       <c r="R4" s="99"/>
-      <c r="S4" s="151" t="s">
+      <c r="S4" s="150" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="151"/>
-      <c r="U4" s="151"/>
-      <c r="V4" s="151"/>
+      <c r="T4" s="150"/>
+      <c r="U4" s="150"/>
+      <c r="V4" s="150"/>
       <c r="W4" s="99"/>
       <c r="X4" s="144" t="s">
         <v>29</v>
@@ -17508,7 +17405,7 @@
       </c>
       <c r="C6" s="90" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">IFERROR(IF(MIN(Milestones43524[Start])=0,TODAY(),B11(Milestones43524[Start])),TODAY())</f>
-        <v>44706</v>
+        <v>44710</v>
       </c>
       <c r="D6" s="91"/>
       <c r="E6" s="84"/>
@@ -17517,7 +17414,7 @@
       <c r="H6" s="84"/>
       <c r="I6" s="109" t="str">
         <f ca="1">TEXT(I7,"mmmm")</f>
-        <v>May</v>
+        <v>June</v>
       </c>
       <c r="J6" s="109"/>
       <c r="K6" s="109"/>
@@ -17527,7 +17424,7 @@
       <c r="O6" s="109"/>
       <c r="P6" s="109" t="str">
         <f ca="1">IF(TEXT(P7,"mmmm")=I6,"",TEXT(P7,"mmmm"))</f>
-        <v>June</v>
+        <v/>
       </c>
       <c r="Q6" s="109"/>
       <c r="R6" s="109"/>
@@ -17557,7 +17454,7 @@
       <c r="AJ6" s="109"/>
       <c r="AK6" s="109" t="str">
         <f ca="1">IF(OR(TEXT(AK7,"mmmm")=AD6,TEXT(AK7,"mmmm")=W6,TEXT(AK7,"mmmm")=P6,TEXT(AK7,"mmmm")=I6),"",TEXT(AK7,"mmmm"))</f>
-        <v/>
+        <v>July</v>
       </c>
       <c r="AL6" s="109"/>
       <c r="AM6" s="109"/>
@@ -17567,7 +17464,7 @@
       <c r="AQ6" s="109"/>
       <c r="AR6" s="109" t="str">
         <f ca="1">IF(OR(TEXT(AR7,"mmmm")=AK6,TEXT(AR7,"mmmm")=AD6,TEXT(AR7,"mmmm")=W6,TEXT(AR7,"mmmm")=P6),"",TEXT(AR7,"mmmm"))</f>
-        <v>July</v>
+        <v/>
       </c>
       <c r="AS6" s="109"/>
       <c r="AT6" s="109"/>
@@ -17612,227 +17509,227 @@
       <c r="H7" s="94"/>
       <c r="I7" s="116">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>44711</v>
+        <v>44715</v>
       </c>
       <c r="J7" s="117">
         <f ca="1">I7+1</f>
-        <v>44712</v>
+        <v>44716</v>
       </c>
       <c r="K7" s="117">
         <f t="shared" ref="K7:AX7" ca="1" si="0">J7+1</f>
-        <v>44713</v>
+        <v>44717</v>
       </c>
       <c r="L7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44714</v>
+        <v>44718</v>
       </c>
       <c r="M7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44715</v>
+        <v>44719</v>
       </c>
       <c r="N7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44716</v>
+        <v>44720</v>
       </c>
       <c r="O7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>44717</v>
+        <v>44721</v>
       </c>
       <c r="P7" s="117">
         <f ca="1">O7+1</f>
-        <v>44718</v>
+        <v>44722</v>
       </c>
       <c r="Q7" s="117">
         <f ca="1">P7+1</f>
-        <v>44719</v>
+        <v>44723</v>
       </c>
       <c r="R7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44720</v>
+        <v>44724</v>
       </c>
       <c r="S7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44721</v>
+        <v>44725</v>
       </c>
       <c r="T7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44722</v>
+        <v>44726</v>
       </c>
       <c r="U7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44723</v>
+        <v>44727</v>
       </c>
       <c r="V7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>44724</v>
+        <v>44728</v>
       </c>
       <c r="W7" s="117">
         <f ca="1">V7+1</f>
-        <v>44725</v>
+        <v>44729</v>
       </c>
       <c r="X7" s="117">
         <f ca="1">W7+1</f>
-        <v>44726</v>
+        <v>44730</v>
       </c>
       <c r="Y7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44727</v>
+        <v>44731</v>
       </c>
       <c r="Z7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44728</v>
+        <v>44732</v>
       </c>
       <c r="AA7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44729</v>
+        <v>44733</v>
       </c>
       <c r="AB7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44730</v>
+        <v>44734</v>
       </c>
       <c r="AC7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>44731</v>
+        <v>44735</v>
       </c>
       <c r="AD7" s="117">
         <f ca="1">AC7+1</f>
-        <v>44732</v>
+        <v>44736</v>
       </c>
       <c r="AE7" s="117">
         <f ca="1">AD7+1</f>
-        <v>44733</v>
+        <v>44737</v>
       </c>
       <c r="AF7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44734</v>
+        <v>44738</v>
       </c>
       <c r="AG7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44735</v>
+        <v>44739</v>
       </c>
       <c r="AH7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44736</v>
+        <v>44740</v>
       </c>
       <c r="AI7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44737</v>
+        <v>44741</v>
       </c>
       <c r="AJ7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>44738</v>
+        <v>44742</v>
       </c>
       <c r="AK7" s="117">
         <f ca="1">AJ7+1</f>
-        <v>44739</v>
+        <v>44743</v>
       </c>
       <c r="AL7" s="117">
         <f ca="1">AK7+1</f>
-        <v>44740</v>
+        <v>44744</v>
       </c>
       <c r="AM7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44741</v>
+        <v>44745</v>
       </c>
       <c r="AN7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44742</v>
+        <v>44746</v>
       </c>
       <c r="AO7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44743</v>
+        <v>44747</v>
       </c>
       <c r="AP7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44744</v>
+        <v>44748</v>
       </c>
       <c r="AQ7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>44745</v>
+        <v>44749</v>
       </c>
       <c r="AR7" s="117">
         <f ca="1">AQ7+1</f>
-        <v>44746</v>
+        <v>44750</v>
       </c>
       <c r="AS7" s="117">
         <f ca="1">AR7+1</f>
-        <v>44747</v>
+        <v>44751</v>
       </c>
       <c r="AT7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44748</v>
+        <v>44752</v>
       </c>
       <c r="AU7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44749</v>
+        <v>44753</v>
       </c>
       <c r="AV7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44750</v>
+        <v>44754</v>
       </c>
       <c r="AW7" s="117">
         <f t="shared" ca="1" si="0"/>
-        <v>44751</v>
+        <v>44755</v>
       </c>
       <c r="AX7" s="118">
         <f t="shared" ca="1" si="0"/>
-        <v>44752</v>
+        <v>44756</v>
       </c>
       <c r="AY7" s="117">
         <f ca="1">AX7+1</f>
-        <v>44753</v>
+        <v>44757</v>
       </c>
       <c r="AZ7" s="117">
         <f ca="1">AY7+1</f>
-        <v>44754</v>
+        <v>44758</v>
       </c>
       <c r="BA7" s="117">
         <f t="shared" ref="BA7:BE7" ca="1" si="1">AZ7+1</f>
-        <v>44755</v>
+        <v>44759</v>
       </c>
       <c r="BB7" s="117">
         <f t="shared" ca="1" si="1"/>
-        <v>44756</v>
+        <v>44760</v>
       </c>
       <c r="BC7" s="117">
         <f t="shared" ca="1" si="1"/>
-        <v>44757</v>
+        <v>44761</v>
       </c>
       <c r="BD7" s="117">
         <f t="shared" ca="1" si="1"/>
-        <v>44758</v>
+        <v>44762</v>
       </c>
       <c r="BE7" s="118">
         <f t="shared" ca="1" si="1"/>
-        <v>44759</v>
+        <v>44763</v>
       </c>
       <c r="BF7" s="117">
         <f ca="1">BE7+1</f>
-        <v>44760</v>
+        <v>44764</v>
       </c>
       <c r="BG7" s="117">
         <f ca="1">BF7+1</f>
-        <v>44761</v>
+        <v>44765</v>
       </c>
       <c r="BH7" s="117">
         <f t="shared" ref="BH7:BL7" ca="1" si="2">BG7+1</f>
-        <v>44762</v>
+        <v>44766</v>
       </c>
       <c r="BI7" s="117">
         <f t="shared" ca="1" si="2"/>
-        <v>44763</v>
+        <v>44767</v>
       </c>
       <c r="BJ7" s="117">
         <f t="shared" ca="1" si="2"/>
-        <v>44764</v>
+        <v>44768</v>
       </c>
       <c r="BK7" s="117">
         <f t="shared" ca="1" si="2"/>
-        <v>44765</v>
+        <v>44769</v>
       </c>
       <c r="BL7" s="118">
         <f t="shared" ca="1" si="2"/>
-        <v>44766</v>
+        <v>44770</v>
       </c>
       <c r="BM7" s="99"/>
     </row>
@@ -17926,227 +17823,227 @@
       <c r="H9" s="105"/>
       <c r="I9" s="124" t="str">
         <f t="shared" ref="I9:BL9" ca="1" si="3">LEFT(TEXT(I7,"ddd"),1)</f>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="J9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="K9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="L9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="M9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="N9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="O9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="P9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="Q9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="R9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="S9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="T9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="U9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="V9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="W9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="X9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="Y9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="Z9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AA9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="AB9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="AC9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AD9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="AE9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AF9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="AG9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AH9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="AI9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="AJ9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AK9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="AL9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AM9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="AN9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AO9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="AP9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="AQ9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AR9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="AS9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="AT9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="AU9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="AV9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="AW9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="AX9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="AY9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="AZ9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="BA9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="BB9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="BC9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="BD9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="BE9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="BF9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>F</v>
       </c>
       <c r="BG9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>S</v>
       </c>
       <c r="BH9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>W</v>
+        <v>S</v>
       </c>
       <c r="BI9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>T</v>
+        <v>M</v>
       </c>
       <c r="BJ9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>T</v>
       </c>
       <c r="BK9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>W</v>
       </c>
       <c r="BL9" s="124" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>T</v>
       </c>
       <c r="BM9" s="99"/>
     </row>
@@ -18470,7 +18367,7 @@
       </c>
       <c r="F12" s="69">
         <f ca="1">TODAY()</f>
-        <v>44706</v>
+        <v>44710</v>
       </c>
       <c r="G12" s="70">
         <v>3</v>
@@ -18714,7 +18611,7 @@
       <c r="E13" s="68"/>
       <c r="F13" s="69">
         <f ca="1">TODAY()+5</f>
-        <v>44711</v>
+        <v>44715</v>
       </c>
       <c r="G13" s="70">
         <v>1</v>
@@ -18960,7 +18857,7 @@
       </c>
       <c r="F14" s="69">
         <f ca="1">F12-3</f>
-        <v>44703</v>
+        <v>44707</v>
       </c>
       <c r="G14" s="70">
         <v>10</v>
@@ -19204,7 +19101,7 @@
       <c r="E15" s="68"/>
       <c r="F15" s="69">
         <f ca="1">F12+20</f>
-        <v>44726</v>
+        <v>44730</v>
       </c>
       <c r="G15" s="70">
         <v>1</v>
@@ -19450,7 +19347,7 @@
       </c>
       <c r="F16" s="69">
         <f ca="1">F12+6</f>
-        <v>44712</v>
+        <v>44716</v>
       </c>
       <c r="G16" s="70">
         <v>6</v>
@@ -19933,7 +19830,7 @@
       </c>
       <c r="F18" s="69">
         <f ca="1">F12+6</f>
-        <v>44712</v>
+        <v>44716</v>
       </c>
       <c r="G18" s="70">
         <v>13</v>
@@ -20179,7 +20076,7 @@
       </c>
       <c r="F19" s="69">
         <f ca="1">F18+2</f>
-        <v>44714</v>
+        <v>44718</v>
       </c>
       <c r="G19" s="70">
         <v>9</v>
@@ -20425,7 +20322,7 @@
       </c>
       <c r="F20" s="69">
         <f ca="1">F19+5</f>
-        <v>44719</v>
+        <v>44723</v>
       </c>
       <c r="G20" s="70">
         <v>11</v>
@@ -20669,7 +20566,7 @@
       <c r="E21" s="68"/>
       <c r="F21" s="69">
         <f ca="1">F20+2</f>
-        <v>44721</v>
+        <v>44725</v>
       </c>
       <c r="G21" s="70">
         <v>1</v>
@@ -20911,7 +20808,7 @@
       <c r="E22" s="68"/>
       <c r="F22" s="69">
         <f ca="1">F21+1</f>
-        <v>44722</v>
+        <v>44726</v>
       </c>
       <c r="G22" s="70">
         <v>24</v>
@@ -21392,7 +21289,7 @@
       <c r="E24" s="68"/>
       <c r="F24" s="69">
         <f ca="1">F12+15</f>
-        <v>44721</v>
+        <v>44725</v>
       </c>
       <c r="G24" s="70">
         <v>4</v>
@@ -21636,7 +21533,7 @@
       <c r="E25" s="68"/>
       <c r="F25" s="69">
         <f ca="1">F24+3</f>
-        <v>44724</v>
+        <v>44728</v>
       </c>
       <c r="G25" s="70">
         <v>14</v>
@@ -21880,7 +21777,7 @@
       <c r="E26" s="68"/>
       <c r="F26" s="69">
         <f ca="1">F25+15</f>
-        <v>44739</v>
+        <v>44743</v>
       </c>
       <c r="G26" s="70">
         <v>6</v>
@@ -22124,7 +22021,7 @@
       <c r="E27" s="68"/>
       <c r="F27" s="69">
         <f ca="1">F21+22</f>
-        <v>44743</v>
+        <v>44747</v>
       </c>
       <c r="G27" s="70">
         <v>3</v>
@@ -22368,7 +22265,7 @@
       <c r="E28" s="68"/>
       <c r="F28" s="69">
         <f ca="1">F16</f>
-        <v>44712</v>
+        <v>44716</v>
       </c>
       <c r="G28" s="70">
         <v>19</v>
@@ -22847,7 +22744,7 @@
       <c r="E30" s="68"/>
       <c r="F30" s="69">
         <f ca="1">F27+3</f>
-        <v>44746</v>
+        <v>44750</v>
       </c>
       <c r="G30" s="70">
         <v>15</v>
@@ -23089,7 +22986,7 @@
       <c r="E31" s="68"/>
       <c r="F31" s="69">
         <f ca="1">F30+14</f>
-        <v>44760</v>
+        <v>44764</v>
       </c>
       <c r="G31" s="70">
         <v>5</v>
@@ -23333,7 +23230,7 @@
       <c r="E32" s="68"/>
       <c r="F32" s="69">
         <f ca="1">F31+42</f>
-        <v>44802</v>
+        <v>44806</v>
       </c>
       <c r="G32" s="70">
         <v>1</v>
@@ -24377,56 +24274,56 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL36">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:AM6">
-    <cfRule type="expression" dxfId="12" priority="4">
+    <cfRule type="expression" dxfId="16" priority="4">
       <formula>I$7&lt;=EOMONTH($I$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:BL6">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="15" priority="3">
       <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BL6">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:BL35">
-    <cfRule type="expression" dxfId="9" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="7" stopIfTrue="1">
       <formula>AND($C10="Low Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="8" stopIfTrue="1">
       <formula>AND($C10="High Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="9" stopIfTrue="1">
       <formula>AND($C10="On Track",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
       <formula>AND($C10="Med Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:BL36">
-    <cfRule type="expression" dxfId="4" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="13" stopIfTrue="1">
       <formula>AND(#REF!="Low Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="14" stopIfTrue="1">
       <formula>AND(#REF!="High Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="15" stopIfTrue="1">
       <formula>AND(#REF!="On Track",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="16" stopIfTrue="1">
       <formula>AND(#REF!="Med Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="17" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24553,6 +24450,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="22a266b9fa9a230c5a512669d8b298c3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eddc33fff6b14141ee5c74a0d29ea6a1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -24828,25 +24744,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -24857,6 +24754,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75C87518-DD8E-42CD-8DAC-291A323E849B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24877,18 +24786,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
   <ds:schemaRefs>

</xml_diff>